<commit_message>
Added Purity KPIs to PROD
</commit_message>
<xml_diff>
--- a/Projects/INBEVCO/Data/Template.xlsx
+++ b/Projects/INBEVCO/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Relative Positioning" sheetId="1" state="visible" r:id="rId2"/>
@@ -50,7 +50,7 @@
             <family val="2"/>
             <charset val="177"/>
           </rPr>
-          <t>Name of KPI</t>
+          <t xml:space="preserve">Name of KPI</t>
         </r>
       </text>
     </comment>
@@ -64,7 +64,7 @@
             <family val="2"/>
             <charset val="177"/>
           </rPr>
-          <t>Please enter the primary "instore location", according the the channel in column E</t>
+          <t xml:space="preserve">Please enter the primary "instore location", according the the channel in column E</t>
         </r>
       </text>
     </comment>
@@ -78,7 +78,7 @@
             <family val="2"/>
             <charset val="177"/>
           </rPr>
-          <t>Please enter the EAN code of the SKU you would like to track</t>
+          <t xml:space="preserve">Please enter the EAN code of the SKU you would like to track</t>
         </r>
       </text>
     </comment>
@@ -92,7 +92,7 @@
             <family val="2"/>
             <charset val="177"/>
           </rPr>
-          <t>Please enter the EAN code of the SKU you would like to track</t>
+          <t xml:space="preserve">Please enter the EAN code of the SKU you would like to track</t>
         </r>
       </text>
     </comment>
@@ -106,7 +106,7 @@
             <family val="2"/>
             <charset val="177"/>
           </rPr>
-          <t>Please enter the EAN code of the SKU that will be used as an anchor. 
+          <t xml:space="preserve">Please enter the EAN code of the SKU that will be used as an anchor. 
 The "Tracked SKU" position will be measured in relation to "Anchor SKU" </t>
         </r>
       </text>
@@ -121,7 +121,7 @@
             <family val="2"/>
             <charset val="177"/>
           </rPr>
-          <t>Please enter the EAN code of the SKU that will be used as an anchor. 
+          <t xml:space="preserve">Please enter the EAN code of the SKU that will be used as an anchor. 
 The "Tracked SKU" position will be measured in relation to "Anchor SKU" </t>
         </r>
       </text>
@@ -146,7 +146,7 @@
             <family val="2"/>
             <charset val="177"/>
           </rPr>
-          <t>Naming Convention: 
+          <t xml:space="preserve">Naming Convention: 
 'Brand Name' or 'Brand Varient' at 'in store location' </t>
         </r>
       </text>
@@ -161,7 +161,7 @@
             <family val="2"/>
             <charset val="177"/>
           </rPr>
-          <t>- Only Primary Location!- 
+          <t xml:space="preserve">- Only Primary Location!- 
 - Off trade - usually Main shelf
 - On trade - usually Back Bar</t>
         </r>
@@ -177,7 +177,7 @@
             <family val="2"/>
             <charset val="177"/>
           </rPr>
-          <t>Brand Variant is optional</t>
+          <t xml:space="preserve">Brand Variant is optional</t>
         </r>
       </text>
     </comment>
@@ -186,168 +186,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="54">
-  <si>
-    <t>Above Direction</t>
-  </si>
-  <si>
-    <t>Below Direction</t>
-  </si>
-  <si>
-    <t>Left Direction</t>
-  </si>
-  <si>
-    <t>Right Direction</t>
-  </si>
-  <si>
-    <t>Channel</t>
-  </si>
-  <si>
-    <t>Atomic Name</t>
-  </si>
-  <si>
-    <t>Primary "In store location"</t>
-  </si>
-  <si>
-    <t>Tested Brand Name</t>
-  </si>
-  <si>
-    <t>Tested SKU EAN </t>
-  </si>
-  <si>
-    <t>Anchor Brand Name</t>
-  </si>
-  <si>
-    <t>Anchor SKU EAN</t>
-  </si>
-  <si>
-    <t>Above Allowed? </t>
-  </si>
-  <si>
-    <t>Up to (above) distance (by shelves) </t>
-  </si>
-  <si>
-    <t>Below Allowed?</t>
-  </si>
-  <si>
-    <t>Up to (below) distance (by shelves)</t>
-  </si>
-  <si>
-    <t>Left Allowed?</t>
-  </si>
-  <si>
-    <t>Up to (Left) Distance (by SKU facings) </t>
-  </si>
-  <si>
-    <t>Right allowed? </t>
-  </si>
-  <si>
-    <t>Up to (right) distance (by SKU facings) </t>
-  </si>
-  <si>
-    <t>Off Trade</t>
-  </si>
-  <si>
-    <t>CLUB COLOMBIA DORADA Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>CLUB COLOMBIA DORADA</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>AGUILA LIGHT Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>AGUILA LIGHT</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>AGUILA  Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>AGUILA </t>
-  </si>
-  <si>
-    <t>POKER Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>POKER</t>
-  </si>
-  <si>
-    <t>Brand Blocking - Template</t>
-  </si>
-  <si>
-    <t>Brand Name</t>
-  </si>
-  <si>
-    <t>Brand Variant</t>
-  </si>
-  <si>
-    <t>CLUB COLOMBIA DORADA At Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>CLUB COLOMBIA ROJA At Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>CLUB COLOMBIA ROJA</t>
-  </si>
-  <si>
-    <t>CLUB COLOMBIA NEGRA At Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>CLUB COLOMBIA NEGRA</t>
-  </si>
-  <si>
-    <t>AGUILA LIGHT At Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>AGUILA At Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>AGUILA</t>
-  </si>
-  <si>
-    <t>POKER At Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>PILSEN At Nevera Bavaria</t>
-  </si>
-  <si>
-    <t>PILSEN</t>
-  </si>
-  <si>
-    <t>Entity Type To Check Purity</t>
-  </si>
-  <si>
-    <t>Value (as Appears in DB)</t>
-  </si>
-  <si>
-    <t>SOS Target to Determine Purity</t>
-  </si>
-  <si>
-    <t>manufacturer_name</t>
-  </si>
-  <si>
-    <t>AB-INBEV</t>
-  </si>
-  <si>
-    <t>Equipo de frio – Disponibilidad</t>
-  </si>
-  <si>
-    <t>Equipos de Frío 2018</t>
-  </si>
-  <si>
-    <t>Disponibilidad NABs</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="57">
+  <si>
+    <t xml:space="preserve">Above Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Below Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atomic Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary "In store location"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tested Brand Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tested SKU EAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anchor Brand Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anchor SKU EAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Above Allowed? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up to (above) distance (by shelves) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Below Allowed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up to (below) distance (by shelves)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Allowed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up to (Left) Distance (by SKU facings) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right allowed? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up to (right) distance (by SKU facings) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off Trade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUB COLOMBIA DORADA Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUB COLOMBIA DORADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGUILA LIGHT Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGUILA LIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGUILA  Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGUILA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POKER Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POKER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand Blocking - Template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand Variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUB COLOMBIA DORADA At Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUB COLOMBIA ROJA At Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUB COLOMBIA ROJA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUB COLOMBIA NEGRA At Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUB COLOMBIA NEGRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGUILA LIGHT At Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGUILA At Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGUILA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POKER At Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PILSEN At Nevera Bavaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PILSEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity Type To Check Purity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value (as Appears in DB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS Target to Determine Purity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manufacturer_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB-INBEV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipo de frio – Disponibilidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipos de Frío 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disponibilidad NABs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevera Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevera Propia/Competencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevera Propia/Competencia - NUEVA</t>
   </si>
 </sst>
 </file>
@@ -355,7 +364,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
@@ -505,7 +514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -576,27 +585,6 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -626,7 +614,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -731,20 +719,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -831,9 +815,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>145440</xdr:rowOff>
+      <xdr:rowOff>145080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -842,13 +826,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="39573" t="2512" r="34487" b="0"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5761080" y="1823040"/>
-          <a:ext cx="1905840" cy="6681240"/>
+        <a:srcRect l="39567" t="2512" r="34481" b="0"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5799240" y="1823040"/>
+          <a:ext cx="1924560" cy="6680880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -869,9 +853,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:rowOff>66240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -885,8 +869,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7405560" y="2966040"/>
-          <a:ext cx="261360" cy="887400"/>
+          <a:off x="7443720" y="2966040"/>
+          <a:ext cx="280080" cy="887040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -907,9 +891,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>804600</xdr:colOff>
+      <xdr:colOff>804240</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -923,8 +907,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6328080" y="3011760"/>
-          <a:ext cx="210240" cy="887400"/>
+          <a:off x="6366240" y="3011760"/>
+          <a:ext cx="209880" cy="887040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -945,9 +929,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>551880</xdr:colOff>
+      <xdr:colOff>551520</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -961,8 +945,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6075360" y="3011760"/>
-          <a:ext cx="210240" cy="887400"/>
+          <a:off x="6113520" y="3011760"/>
+          <a:ext cx="209880" cy="887040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -983,9 +967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1700640</xdr:colOff>
+      <xdr:colOff>1700280</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>53280</xdr:rowOff>
+      <xdr:rowOff>52920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -999,8 +983,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7172640" y="2952720"/>
-          <a:ext cx="261720" cy="887400"/>
+          <a:off x="7210800" y="2952720"/>
+          <a:ext cx="261360" cy="887040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1021,9 +1005,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>783720</xdr:colOff>
+      <xdr:colOff>783360</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:rowOff>77760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1036,8 +1020,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6293520" y="4799880"/>
-          <a:ext cx="223920" cy="779760"/>
+          <a:off x="6331680" y="4799880"/>
+          <a:ext cx="223560" cy="779400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1058,9 +1042,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>508680</xdr:colOff>
+      <xdr:colOff>508320</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:rowOff>77760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1073,8 +1057,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6018480" y="4799880"/>
-          <a:ext cx="223920" cy="779760"/>
+          <a:off x="6056640" y="4799880"/>
+          <a:ext cx="223560" cy="779400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1095,9 +1079,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1074600</xdr:colOff>
+      <xdr:colOff>1074240</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1110,8 +1094,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6584400" y="4804560"/>
-          <a:ext cx="223920" cy="779760"/>
+          <a:off x="6622560" y="4804560"/>
+          <a:ext cx="223560" cy="779400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1132,9 +1116,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1147,8 +1131,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7482960" y="4797720"/>
-          <a:ext cx="183960" cy="779760"/>
+          <a:off x="7521120" y="4797720"/>
+          <a:ext cx="202680" cy="779400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1169,9 +1153,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1382400</xdr:colOff>
+      <xdr:colOff>1382040</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1184,8 +1168,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6892200" y="4804560"/>
-          <a:ext cx="223920" cy="779760"/>
+          <a:off x="6930360" y="4804560"/>
+          <a:ext cx="223560" cy="779400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1206,9 +1190,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1676160</xdr:colOff>
+      <xdr:colOff>1675800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1221,8 +1205,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7185960" y="4804560"/>
-          <a:ext cx="223920" cy="779760"/>
+          <a:off x="7224120" y="4804560"/>
+          <a:ext cx="223560" cy="779400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1243,9 +1227,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>821880</xdr:colOff>
+      <xdr:colOff>821520</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>45360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1258,8 +1242,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6319440" y="3961800"/>
-          <a:ext cx="236160" cy="823320"/>
+          <a:off x="6357600" y="3961800"/>
+          <a:ext cx="235800" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1280,9 +1264,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>559800</xdr:colOff>
+      <xdr:colOff>559440</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1295,8 +1279,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6057360" y="3953160"/>
-          <a:ext cx="236160" cy="823320"/>
+          <a:off x="6095520" y="3953160"/>
+          <a:ext cx="235800" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1317,9 +1301,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1106280</xdr:colOff>
+      <xdr:colOff>1105920</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1332,8 +1316,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6603840" y="3949200"/>
-          <a:ext cx="236160" cy="823320"/>
+          <a:off x="6642000" y="3949200"/>
+          <a:ext cx="235800" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1354,9 +1338,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:rowOff>26280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1369,8 +1353,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7502400" y="3942720"/>
-          <a:ext cx="164520" cy="823320"/>
+          <a:off x="7540560" y="3942720"/>
+          <a:ext cx="183240" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1391,9 +1375,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1414080</xdr:colOff>
+      <xdr:colOff>1413720</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1406,8 +1390,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6911640" y="3949200"/>
-          <a:ext cx="236160" cy="823320"/>
+          <a:off x="6949800" y="3949200"/>
+          <a:ext cx="235800" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1428,9 +1412,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1707480</xdr:colOff>
+      <xdr:colOff>1707120</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1443,8 +1427,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7205040" y="3949200"/>
-          <a:ext cx="236160" cy="823320"/>
+          <a:off x="7243200" y="3949200"/>
+          <a:ext cx="235800" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1465,9 +1449,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>508680</xdr:colOff>
+      <xdr:colOff>508320</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1481,8 +1465,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6009840" y="5595840"/>
-          <a:ext cx="232560" cy="771480"/>
+          <a:off x="6048000" y="5595840"/>
+          <a:ext cx="232200" cy="771120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1503,9 +1487,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>798840</xdr:colOff>
+      <xdr:colOff>798480</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
+      <xdr:rowOff>116640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1519,8 +1503,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6300000" y="5609160"/>
-          <a:ext cx="232560" cy="771480"/>
+          <a:off x="6338160" y="5609160"/>
+          <a:ext cx="232200" cy="771120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1541,9 +1525,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1069200</xdr:colOff>
+      <xdr:colOff>1068840</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
+      <xdr:rowOff>116640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1557,8 +1541,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6570360" y="5609160"/>
-          <a:ext cx="232560" cy="771480"/>
+          <a:off x="6608520" y="5609160"/>
+          <a:ext cx="232200" cy="771120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1579,9 +1563,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1405800</xdr:colOff>
+      <xdr:colOff>1405440</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>93240</xdr:rowOff>
+      <xdr:rowOff>92880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1595,8 +1579,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6919560" y="5586840"/>
-          <a:ext cx="219960" cy="770040"/>
+          <a:off x="6957720" y="5586840"/>
+          <a:ext cx="219600" cy="769680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1617,9 +1601,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1715760</xdr:colOff>
+      <xdr:colOff>1715400</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1633,8 +1617,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7204680" y="6452280"/>
-          <a:ext cx="244800" cy="770400"/>
+          <a:off x="7242840" y="6452280"/>
+          <a:ext cx="244440" cy="770040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1655,9 +1639,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1691280</xdr:colOff>
+      <xdr:colOff>1690920</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1671,8 +1655,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7205040" y="5580000"/>
-          <a:ext cx="219960" cy="770040"/>
+          <a:off x="7243200" y="5580000"/>
+          <a:ext cx="219600" cy="769680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1693,9 +1677,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>82440</xdr:rowOff>
+      <xdr:rowOff>82080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1709,8 +1693,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7502400" y="5576040"/>
-          <a:ext cx="164520" cy="770040"/>
+          <a:off x="7540560" y="5576040"/>
+          <a:ext cx="183240" cy="769680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1731,9 +1715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>813600</xdr:colOff>
+      <xdr:colOff>813240</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:rowOff>26280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1747,8 +1731,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6327360" y="6472080"/>
-          <a:ext cx="219960" cy="770400"/>
+          <a:off x="6365520" y="6472080"/>
+          <a:ext cx="219600" cy="770040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1769,9 +1753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>551520</xdr:colOff>
+      <xdr:colOff>551160</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
+      <xdr:rowOff>27000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1785,8 +1769,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6065280" y="6472800"/>
-          <a:ext cx="219960" cy="770400"/>
+          <a:off x="6103440" y="6472800"/>
+          <a:ext cx="219600" cy="770040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1807,9 +1791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1823,8 +1807,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7459560" y="6466320"/>
-          <a:ext cx="207360" cy="770400"/>
+          <a:off x="7497720" y="6466320"/>
+          <a:ext cx="226080" cy="770040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1845,9 +1829,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1449720</xdr:colOff>
+      <xdr:colOff>1449360</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1861,8 +1845,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6938640" y="6454440"/>
-          <a:ext cx="244800" cy="770400"/>
+          <a:off x="6976800" y="6454440"/>
+          <a:ext cx="244440" cy="770040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1883,9 +1867,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1112760</xdr:colOff>
+      <xdr:colOff>1112400</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1899,8 +1883,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6626520" y="6455520"/>
-          <a:ext cx="219960" cy="770400"/>
+          <a:off x="6664680" y="6455520"/>
+          <a:ext cx="219600" cy="770040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1921,9 +1905,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1092960</xdr:colOff>
+      <xdr:colOff>1092600</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1937,8 +1921,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6616440" y="3000960"/>
-          <a:ext cx="210240" cy="887400"/>
+          <a:off x="6654600" y="3000960"/>
+          <a:ext cx="209880" cy="887040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1959,9 +1943,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1417680</xdr:colOff>
+      <xdr:colOff>1417320</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1975,8 +1959,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6889680" y="2955240"/>
-          <a:ext cx="261720" cy="887400"/>
+          <a:off x="6927840" y="2955240"/>
+          <a:ext cx="261360" cy="887040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2000,23 +1984,23 @@
   <dimension ref="B2:P65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="1" sqref="B6:E8 G20"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="1" sqref="B9:E11 G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.6396761133603"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8542510121457"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="3.10526315789474"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="1.71255060728745"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="1.60728744939271"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.74898785425101"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="2.03643724696356"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="1.92712550607287"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.10526315789474"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.10526315789474"/>
@@ -2305,63 +2289,63 @@
   <dimension ref="B1:F14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="1" sqref="B6:E8 D22"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="1" sqref="B9:E11 D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.3117408906883"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="253" min="10" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="254" min="254" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="255" min="255" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="256" min="256" style="0" width="75.7327935222672"/>
+    <col collapsed="false" hidden="false" max="255" min="255" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="256" min="256" style="0" width="76.4817813765182"/>
     <col collapsed="false" hidden="false" max="257" min="257" style="0" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="258" min="258" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="259" min="259" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="259" min="259" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="262" min="262" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="263" min="263" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="264" min="264" style="0" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="265" min="265" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="264" min="264" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="265" min="265" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="509" min="266" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="510" min="510" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="511" min="511" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="512" min="512" style="0" width="75.7327935222672"/>
+    <col collapsed="false" hidden="false" max="511" min="511" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="512" min="512" style="0" width="76.4817813765182"/>
     <col collapsed="false" hidden="false" max="513" min="513" style="0" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="514" min="514" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="515" min="515" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="516" min="516" style="0" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="517" min="517" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="515" min="515" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="516" min="516" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="517" min="517" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="518" min="518" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="519" min="519" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="520" min="520" style="0" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="521" min="521" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="520" min="520" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="521" min="521" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="765" min="522" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="766" min="766" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="767" min="767" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="768" min="768" style="0" width="75.7327935222672"/>
+    <col collapsed="false" hidden="false" max="767" min="767" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="768" min="768" style="0" width="76.4817813765182"/>
     <col collapsed="false" hidden="false" max="769" min="769" style="0" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="770" min="770" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="771" min="771" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="772" min="772" style="0" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="773" min="773" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="771" min="771" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="772" min="772" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="773" min="773" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="774" min="774" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="775" min="775" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="776" min="776" style="0" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="777" min="777" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="776" min="776" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="777" min="777" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="1021" min="778" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1022" min="1022" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="1023" min="1023" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="75.7327935222672"/>
+    <col collapsed="false" hidden="false" max="1023" min="1023" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="76.4817813765182"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2542,19 +2526,19 @@
     <tabColor rgb="FFDAE3F3"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6:E8"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2635,11 +2619,47 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
+    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="25" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="25" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="25" t="n">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>